<commit_message>
RR test link added
</commit_message>
<xml_diff>
--- a/Links/DLD_Links.xlsx
+++ b/Links/DLD_Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GATE\GATE_CS_2021\Links\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13DC981-0F4A-4F95-AD82-35377573404B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B689A2C-0F09-464C-971D-84BF7E000FF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Chapter</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>Links</t>
+  </si>
+  <si>
+    <t>Combinational Circuits</t>
+  </si>
+  <si>
+    <t>NOR (Half Add/Sub)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=P_UW41wMvpM</t>
   </si>
 </sst>
 </file>
@@ -104,11 +113,11 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -391,37 +400,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
@@ -432,12 +441,23 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>